<commit_message>
fix(file): US -> USD
</commit_message>
<xml_diff>
--- a/data/xls/eco/VCA4D Coffee Ecuador Transfer.xlsx
+++ b/data/xls/eco/VCA4D Coffee Ecuador Transfer.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="171">
   <si>
     <t xml:space="preserve">Property</t>
   </si>
@@ -64,13 +64,10 @@
     <t xml:space="preserve">Study's local currency</t>
   </si>
   <si>
-    <t xml:space="preserve">US</t>
+    <t xml:space="preserve">USD</t>
   </si>
   <si>
     <t xml:space="preserve">Standard currency code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USD</t>
   </si>
   <si>
     <t xml:space="preserve">change rate from study's to standard currency</t>
@@ -665,11 +662,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -688,17 +685,17 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>146</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -706,7 +703,7 @@
         <v>186</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>5841818.16543232</v>
@@ -717,7 +714,7 @@
         <v>187</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>729927.234903763</v>
@@ -728,7 +725,7 @@
         <v>188</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>621430.271428541</v>
@@ -739,7 +736,7 @@
         <v>191</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>293502.198874323</v>
@@ -750,7 +747,7 @@
         <v>192</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>2724539.08577526</v>
@@ -761,7 +758,7 @@
         <v>193</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>12271410.4190476</v>
@@ -772,7 +769,7 @@
         <v>195</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>6101463.23162832</v>
@@ -783,7 +780,7 @@
         <v>196</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>136646.465550005</v>
@@ -794,7 +791,7 @@
         <v>197</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>830641.433828528</v>
@@ -805,7 +802,7 @@
         <v>198</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>679657.000221099</v>
@@ -816,7 +813,7 @@
         <v>199</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>25846547.4870402</v>
@@ -824,7 +821,7 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>0</v>
@@ -832,7 +829,7 @@
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>11979570.8198526</v>
@@ -840,7 +837,7 @@
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>15651653.0923037</v>
@@ -848,7 +845,7 @@
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>0</v>
@@ -856,7 +853,7 @@
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>174805.067685938</v>
@@ -864,8 +861,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -884,47 +881,47 @@
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.45"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="51.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>2</v>
@@ -932,195 +929,195 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>152.212275372031</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>389.17165075149</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>72.9696845159044</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>1853.51708447574</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>347.534453339202</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>49.2784362898615</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>9.23970680434903</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>0</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>12.2791423001949</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>21.4084507042254</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>75.9277176823765</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>14.2364470654456</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" s="2" t="n">
         <v>265.901360644419</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F12" s="2" t="n">
         <v>49.8565051208285</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1139,20 +1136,20 @@
       <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="0" t="s">
         <v>160</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>161</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>1</v>
@@ -1163,13 +1160,13 @@
         <v>186</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>2654590.92547677</v>
@@ -1180,13 +1177,13 @@
         <v>187</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>74503.0838454333</v>
@@ -1197,13 +1194,13 @@
         <v>188</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>4199866.66666666</v>
@@ -1214,13 +1211,13 @@
         <v>189</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>0</v>
@@ -1231,13 +1228,13 @@
         <v>190</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>0</v>
@@ -1248,13 +1245,13 @@
         <v>191</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>44941.6607747998</v>
@@ -1265,13 +1262,13 @@
         <v>192</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>1367335.54657768</v>
@@ -1282,13 +1279,13 @@
         <v>193</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>277491.19047619</v>
@@ -1299,13 +1296,13 @@
         <v>194</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>0</v>
@@ -1316,13 +1313,13 @@
         <v>195</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>2125537.02607567</v>
@@ -1333,13 +1330,13 @@
         <v>196</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>16932.4121811021</v>
@@ -1350,13 +1347,13 @@
         <v>197</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>83414.77565273</v>
@@ -1367,13 +1364,13 @@
         <v>198</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>121315.391657326</v>
@@ -1384,13 +1381,13 @@
         <v>199</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>1013642.14046823</v>
@@ -1401,13 +1398,13 @@
         <v>200</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>0</v>
@@ -1418,13 +1415,13 @@
         <v>201</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>0</v>
@@ -1435,13 +1432,13 @@
         <v>186</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D18" s="0" t="s">
         <v>162</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>163</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>721636.363636364</v>
@@ -1452,13 +1449,13 @@
         <v>187</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C19" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D19" s="0" t="s">
         <v>162</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>163</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>14908632.0347334</v>
@@ -1469,13 +1466,13 @@
         <v>188</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C20" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D20" s="0" t="s">
         <v>162</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>163</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>8409723.01619047</v>
@@ -1486,13 +1483,13 @@
         <v>189</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C21" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D21" s="0" t="s">
         <v>162</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>163</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>0</v>
@@ -1503,13 +1500,13 @@
         <v>190</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D22" s="0" t="s">
         <v>162</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>163</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>0</v>
@@ -1520,13 +1517,13 @@
         <v>191</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D23" s="0" t="s">
         <v>162</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>163</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>4330700</v>
@@ -1537,13 +1534,13 @@
         <v>192</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C24" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D24" s="0" t="s">
         <v>162</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>163</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>65134.1911764706</v>
@@ -1554,13 +1551,13 @@
         <v>193</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C25" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D25" s="0" t="s">
         <v>162</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>163</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>8315736</v>
@@ -1571,13 +1568,13 @@
         <v>194</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C26" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D26" s="0" t="s">
         <v>162</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>163</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>0</v>
@@ -1588,13 +1585,13 @@
         <v>195</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C27" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D27" s="0" t="s">
         <v>162</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>163</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>237500</v>
@@ -1605,13 +1602,13 @@
         <v>196</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C28" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D28" s="0" t="s">
         <v>162</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>163</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>8466667.60548068</v>
@@ -1622,13 +1619,13 @@
         <v>197</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C29" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D29" s="0" t="s">
         <v>162</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>163</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>9241024.29796303</v>
@@ -1639,13 +1636,13 @@
         <v>198</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C30" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D30" s="0" t="s">
         <v>162</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>163</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>11431890.9006974</v>
@@ -1656,13 +1653,13 @@
         <v>199</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C31" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D31" s="0" t="s">
         <v>162</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>163</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>84951227.5965719</v>
@@ -1673,13 +1670,13 @@
         <v>200</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C32" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D32" s="0" t="s">
         <v>162</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>163</v>
       </c>
       <c r="E32" s="0" t="n">
         <v>0</v>
@@ -1690,13 +1687,13 @@
         <v>201</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C33" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D33" s="0" t="s">
         <v>162</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>163</v>
       </c>
       <c r="E33" s="0" t="n">
         <v>0</v>
@@ -1707,13 +1704,13 @@
         <v>186</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E34" s="0" t="n">
         <v>0</v>
@@ -1724,13 +1721,13 @@
         <v>187</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>0</v>
@@ -1741,13 +1738,13 @@
         <v>188</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E36" s="0" t="n">
         <v>0</v>
@@ -1758,13 +1755,13 @@
         <v>189</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E37" s="0" t="n">
         <v>0</v>
@@ -1775,13 +1772,13 @@
         <v>190</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E38" s="0" t="n">
         <v>0</v>
@@ -1792,13 +1789,13 @@
         <v>191</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E39" s="0" t="n">
         <v>0</v>
@@ -1809,13 +1806,13 @@
         <v>192</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E40" s="0" t="n">
         <v>0</v>
@@ -1826,13 +1823,13 @@
         <v>193</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E41" s="0" t="n">
         <v>0</v>
@@ -1843,13 +1840,13 @@
         <v>194</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E42" s="0" t="n">
         <v>0</v>
@@ -1860,13 +1857,13 @@
         <v>195</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E43" s="0" t="n">
         <v>0</v>
@@ -1877,13 +1874,13 @@
         <v>196</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E44" s="0" t="n">
         <v>0</v>
@@ -1894,13 +1891,13 @@
         <v>197</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E45" s="0" t="n">
         <v>0</v>
@@ -1911,13 +1908,13 @@
         <v>198</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E46" s="0" t="n">
         <v>0</v>
@@ -1928,13 +1925,13 @@
         <v>199</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E47" s="0" t="n">
         <v>0</v>
@@ -1945,13 +1942,13 @@
         <v>200</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E48" s="0" t="n">
         <v>0</v>
@@ -1962,13 +1959,13 @@
         <v>201</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E49" s="0" t="n">
         <v>0</v>
@@ -1979,13 +1976,13 @@
         <v>186</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E50" s="0" t="n">
         <v>0</v>
@@ -1996,13 +1993,13 @@
         <v>187</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E51" s="0" t="n">
         <v>0</v>
@@ -2013,13 +2010,13 @@
         <v>188</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E52" s="0" t="n">
         <v>0</v>
@@ -2030,13 +2027,13 @@
         <v>189</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E53" s="0" t="n">
         <v>0</v>
@@ -2047,13 +2044,13 @@
         <v>190</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E54" s="0" t="n">
         <v>0</v>
@@ -2064,13 +2061,13 @@
         <v>191</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E55" s="0" t="n">
         <v>0</v>
@@ -2081,13 +2078,13 @@
         <v>192</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E56" s="0" t="n">
         <v>0</v>
@@ -2098,13 +2095,13 @@
         <v>193</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E57" s="0" t="n">
         <v>0</v>
@@ -2115,13 +2112,13 @@
         <v>194</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E58" s="0" t="n">
         <v>0</v>
@@ -2132,13 +2129,13 @@
         <v>195</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E59" s="0" t="n">
         <v>0</v>
@@ -2149,13 +2146,13 @@
         <v>196</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E60" s="0" t="n">
         <v>0</v>
@@ -2166,13 +2163,13 @@
         <v>197</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E61" s="0" t="n">
         <v>0</v>
@@ -2183,13 +2180,13 @@
         <v>198</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E62" s="0" t="n">
         <v>0</v>
@@ -2200,13 +2197,13 @@
         <v>199</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E63" s="0" t="n">
         <v>0</v>
@@ -2217,13 +2214,13 @@
         <v>200</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E64" s="0" t="n">
         <v>0</v>
@@ -2234,13 +2231,13 @@
         <v>201</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E65" s="0" t="n">
         <v>0</v>
@@ -2251,13 +2248,13 @@
         <v>186</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E66" s="0" t="n">
         <v>5841818.16543232</v>
@@ -2268,13 +2265,13 @@
         <v>187</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E67" s="0" t="n">
         <v>729927.234903794</v>
@@ -2285,13 +2282,13 @@
         <v>188</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E68" s="0" t="n">
         <v>621430.271428574</v>
@@ -2302,13 +2299,13 @@
         <v>189</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E69" s="0" t="n">
         <v>0</v>
@@ -2319,13 +2316,13 @@
         <v>190</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E70" s="0" t="n">
         <v>0</v>
@@ -2336,13 +2333,13 @@
         <v>191</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E71" s="0" t="n">
         <v>293502.198874323</v>
@@ -2353,13 +2350,13 @@
         <v>192</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E72" s="0" t="n">
         <v>2724539.08577526</v>
@@ -2370,13 +2367,13 @@
         <v>193</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E73" s="0" t="n">
         <v>12271410.4190476</v>
@@ -2387,13 +2384,13 @@
         <v>194</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E74" s="0" t="n">
         <v>0</v>
@@ -2404,13 +2401,13 @@
         <v>195</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E75" s="0" t="n">
         <v>6101463.23162832</v>
@@ -2421,13 +2418,13 @@
         <v>196</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E76" s="0" t="n">
         <v>136646.465550007</v>
@@ -2438,13 +2435,13 @@
         <v>197</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E77" s="0" t="n">
         <v>830641.433828549</v>
@@ -2455,13 +2452,13 @@
         <v>198</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E78" s="0" t="n">
         <v>679657.000221048</v>
@@ -2472,13 +2469,13 @@
         <v>199</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E79" s="0" t="n">
         <v>25846547.4870402</v>
@@ -2489,13 +2486,13 @@
         <v>200</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E80" s="0" t="n">
         <v>0</v>
@@ -2506,13 +2503,13 @@
         <v>201</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E81" s="0" t="n">
         <v>0</v>
@@ -2523,13 +2520,13 @@
         <v>186</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C82" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D82" s="0" t="s">
         <v>167</v>
-      </c>
-      <c r="D82" s="0" t="s">
-        <v>168</v>
       </c>
       <c r="E82" s="0" t="n">
         <v>9355500</v>
@@ -2540,13 +2537,13 @@
         <v>187</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C83" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D83" s="0" t="s">
         <v>167</v>
-      </c>
-      <c r="D83" s="0" t="s">
-        <v>168</v>
       </c>
       <c r="E83" s="0" t="n">
         <v>16631472</v>
@@ -2557,13 +2554,13 @@
         <v>188</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C84" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D84" s="0" t="s">
         <v>167</v>
-      </c>
-      <c r="D84" s="0" t="s">
-        <v>168</v>
       </c>
       <c r="E84" s="0" t="n">
         <v>15464509.047619</v>
@@ -2574,13 +2571,13 @@
         <v>189</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C85" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D85" s="0" t="s">
         <v>167</v>
-      </c>
-      <c r="D85" s="0" t="s">
-        <v>168</v>
       </c>
       <c r="E85" s="0" t="n">
         <v>0</v>
@@ -2591,13 +2588,13 @@
         <v>190</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C86" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D86" s="0" t="s">
         <v>167</v>
-      </c>
-      <c r="D86" s="0" t="s">
-        <v>168</v>
       </c>
       <c r="E86" s="0" t="n">
         <v>0</v>
@@ -2608,13 +2605,13 @@
         <v>191</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C87" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D87" s="0" t="s">
         <v>167</v>
-      </c>
-      <c r="D87" s="0" t="s">
-        <v>168</v>
       </c>
       <c r="E87" s="0" t="n">
         <v>4724400</v>
@@ -2625,13 +2622,13 @@
         <v>192</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C88" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D88" s="0" t="s">
         <v>167</v>
-      </c>
-      <c r="D88" s="0" t="s">
-        <v>168</v>
       </c>
       <c r="E88" s="0" t="n">
         <v>4330700</v>
@@ -2642,13 +2639,13 @@
         <v>193</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C89" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D89" s="0" t="s">
         <v>167</v>
-      </c>
-      <c r="D89" s="0" t="s">
-        <v>168</v>
       </c>
       <c r="E89" s="0" t="n">
         <v>21419320</v>
@@ -2659,13 +2656,13 @@
         <v>194</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C90" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D90" s="0" t="s">
         <v>167</v>
-      </c>
-      <c r="D90" s="0" t="s">
-        <v>168</v>
       </c>
       <c r="E90" s="0" t="n">
         <v>0</v>
@@ -2676,13 +2673,13 @@
         <v>195</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C91" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D91" s="0" t="s">
         <v>167</v>
-      </c>
-      <c r="D91" s="0" t="s">
-        <v>168</v>
       </c>
       <c r="E91" s="0" t="n">
         <v>8464500.25770399</v>
@@ -2693,13 +2690,13 @@
         <v>196</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C92" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D92" s="0" t="s">
         <v>167</v>
-      </c>
-      <c r="D92" s="0" t="s">
-        <v>168</v>
       </c>
       <c r="E92" s="0" t="n">
         <v>8778000</v>
@@ -2710,13 +2707,13 @@
         <v>197</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C93" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D93" s="0" t="s">
         <v>167</v>
-      </c>
-      <c r="D93" s="0" t="s">
-        <v>168</v>
       </c>
       <c r="E93" s="0" t="n">
         <v>11000380.4347826</v>
@@ -2727,13 +2724,13 @@
         <v>198</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C94" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D94" s="0" t="s">
         <v>167</v>
-      </c>
-      <c r="D94" s="0" t="s">
-        <v>168</v>
       </c>
       <c r="E94" s="0" t="n">
         <v>13754347.826087</v>
@@ -2744,13 +2741,13 @@
         <v>199</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C95" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D95" s="0" t="s">
         <v>167</v>
-      </c>
-      <c r="D95" s="0" t="s">
-        <v>168</v>
       </c>
       <c r="E95" s="0" t="n">
         <v>122490861.204013</v>
@@ -2761,13 +2758,13 @@
         <v>200</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C96" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D96" s="0" t="s">
         <v>167</v>
-      </c>
-      <c r="D96" s="0" t="s">
-        <v>168</v>
       </c>
       <c r="E96" s="0" t="n">
         <v>0</v>
@@ -2778,13 +2775,13 @@
         <v>201</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C97" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D97" s="0" t="s">
         <v>167</v>
-      </c>
-      <c r="D97" s="0" t="s">
-        <v>168</v>
       </c>
       <c r="E97" s="0" t="n">
         <v>0</v>
@@ -2795,13 +2792,13 @@
         <v>186</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E98" s="0" t="n">
         <v>0</v>
@@ -2812,13 +2809,13 @@
         <v>187</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E99" s="0" t="n">
         <v>0</v>
@@ -2829,13 +2826,13 @@
         <v>188</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E100" s="0" t="n">
         <v>0</v>
@@ -2846,13 +2843,13 @@
         <v>189</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E101" s="0" t="n">
         <v>0</v>
@@ -2863,13 +2860,13 @@
         <v>190</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E102" s="0" t="n">
         <v>0</v>
@@ -2880,13 +2877,13 @@
         <v>191</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E103" s="0" t="n">
         <v>0</v>
@@ -2897,13 +2894,13 @@
         <v>192</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E104" s="0" t="n">
         <v>0</v>
@@ -2914,13 +2911,13 @@
         <v>193</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D105" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E105" s="0" t="n">
         <v>0</v>
@@ -2931,13 +2928,13 @@
         <v>194</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D106" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E106" s="0" t="n">
         <v>0</v>
@@ -2948,13 +2945,13 @@
         <v>195</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D107" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E107" s="0" t="n">
         <v>0</v>
@@ -2965,13 +2962,13 @@
         <v>196</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D108" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E108" s="0" t="n">
         <v>0</v>
@@ -2982,13 +2979,13 @@
         <v>197</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E109" s="0" t="n">
         <v>0</v>
@@ -2999,13 +2996,13 @@
         <v>198</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E110" s="0" t="n">
         <v>0</v>
@@ -3016,13 +3013,13 @@
         <v>199</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E111" s="0" t="n">
         <v>0</v>
@@ -3033,13 +3030,13 @@
         <v>200</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E112" s="0" t="n">
         <v>0</v>
@@ -3050,13 +3047,13 @@
         <v>201</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E113" s="0" t="n">
         <v>0</v>
@@ -3067,13 +3064,13 @@
         <v>186</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E114" s="0" t="n">
         <v>0</v>
@@ -3084,13 +3081,13 @@
         <v>187</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E115" s="0" t="n">
         <v>0</v>
@@ -3101,13 +3098,13 @@
         <v>188</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E116" s="0" t="n">
         <v>29999.0476190476</v>
@@ -3118,13 +3115,13 @@
         <v>189</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E117" s="0" t="n">
         <v>0</v>
@@ -3135,13 +3132,13 @@
         <v>190</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D118" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E118" s="0" t="n">
         <v>0</v>
@@ -3152,13 +3149,13 @@
         <v>191</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E119" s="0" t="n">
         <v>0</v>
@@ -3169,13 +3166,13 @@
         <v>192</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D120" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E120" s="0" t="n">
         <v>0</v>
@@ -3186,13 +3183,13 @@
         <v>193</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D121" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E121" s="0" t="n">
         <v>0</v>
@@ -3203,13 +3200,13 @@
         <v>194</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D122" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E122" s="0" t="n">
         <v>0</v>
@@ -3220,13 +3217,13 @@
         <v>195</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D123" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E123" s="0" t="n">
         <v>0</v>
@@ -3237,13 +3234,13 @@
         <v>196</v>
       </c>
       <c r="B124" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D124" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E124" s="0" t="n">
         <v>0</v>
@@ -3254,13 +3251,13 @@
         <v>197</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D125" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E125" s="0" t="n">
         <v>0</v>
@@ -3271,13 +3268,13 @@
         <v>198</v>
       </c>
       <c r="B126" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D126" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E126" s="0" t="n">
         <v>0</v>
@@ -3288,13 +3285,13 @@
         <v>199</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D127" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E127" s="0" t="n">
         <v>144806.02006689</v>
@@ -3305,13 +3302,13 @@
         <v>200</v>
       </c>
       <c r="B128" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D128" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E128" s="0" t="n">
         <v>0</v>
@@ -3322,13 +3319,13 @@
         <v>201</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D129" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E129" s="0" t="n">
         <v>0</v>
@@ -3339,13 +3336,13 @@
         <v>186</v>
       </c>
       <c r="B130" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D130" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E130" s="0" t="n">
         <v>0</v>
@@ -3356,13 +3353,13 @@
         <v>187</v>
       </c>
       <c r="B131" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D131" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E131" s="0" t="n">
         <v>684955.239174139</v>
@@ -3373,13 +3370,13 @@
         <v>188</v>
       </c>
       <c r="B132" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D132" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E132" s="0" t="n">
         <v>2189090.50285714</v>
@@ -3390,13 +3387,13 @@
         <v>189</v>
       </c>
       <c r="B133" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D133" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E133" s="0" t="n">
         <v>0</v>
@@ -3407,13 +3404,13 @@
         <v>190</v>
       </c>
       <c r="B134" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D134" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E134" s="0" t="n">
         <v>0</v>
@@ -3424,13 +3421,13 @@
         <v>191</v>
       </c>
       <c r="B135" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D135" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E135" s="0" t="n">
         <v>55256.1403508772</v>
@@ -3441,13 +3438,13 @@
         <v>192</v>
       </c>
       <c r="B136" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D136" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E136" s="0" t="n">
         <v>0</v>
@@ -3458,13 +3455,13 @@
         <v>193</v>
       </c>
       <c r="B137" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C137" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D137" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E137" s="0" t="n">
         <v>277191.2</v>
@@ -3475,13 +3472,13 @@
         <v>194</v>
       </c>
       <c r="B138" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D138" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E138" s="0" t="n">
         <v>0</v>
@@ -3492,13 +3489,13 @@
         <v>195</v>
       </c>
       <c r="B139" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D139" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E139" s="0" t="n">
         <v>0</v>
@@ -3509,13 +3506,13 @@
         <v>196</v>
       </c>
       <c r="B140" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D140" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E140" s="0" t="n">
         <v>96338.0281690141</v>
@@ -3526,13 +3523,13 @@
         <v>197</v>
       </c>
       <c r="B141" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D141" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E141" s="0" t="n">
         <v>427093.40559918</v>
@@ -3543,13 +3540,13 @@
         <v>198</v>
       </c>
       <c r="B142" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D142" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E142" s="0" t="n">
         <v>1495695.13133726</v>
@@ -3560,13 +3557,13 @@
         <v>199</v>
       </c>
       <c r="B143" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D143" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E143" s="0" t="n">
         <v>10426033.4448161</v>
@@ -3577,13 +3574,13 @@
         <v>200</v>
       </c>
       <c r="B144" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D144" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E144" s="0" t="n">
         <v>0</v>
@@ -3594,13 +3591,13 @@
         <v>201</v>
       </c>
       <c r="B145" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C145" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D145" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E145" s="0" t="n">
         <v>0</v>
@@ -3608,8 +3605,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3628,11 +3625,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3648,10 +3645,10 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.27"/>
   </cols>
@@ -3711,67 +3708,61 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>15</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>9450</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>7874</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>28500</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1</v>
@@ -3782,84 +3773,84 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>565000</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>85267787</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0.1</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0.9</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>68.5</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0.2</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>12342000</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0.2</v>
@@ -3870,7 +3861,7 @@
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0.82</v>
@@ -3885,8 +3876,8 @@
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3905,53 +3896,53 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3970,7 +3961,7 @@
       <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32"/>
@@ -3978,13 +3969,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3992,10 +3983,10 @@
         <v>186</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4003,10 +3994,10 @@
         <v>187</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4014,10 +4005,10 @@
         <v>188</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4025,10 +4016,10 @@
         <v>189</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4036,10 +4027,10 @@
         <v>190</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>46</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4047,10 +4038,10 @@
         <v>191</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4058,10 +4049,10 @@
         <v>192</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4069,10 +4060,10 @@
         <v>193</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4080,10 +4071,10 @@
         <v>194</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4091,10 +4082,10 @@
         <v>195</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4102,10 +4093,10 @@
         <v>196</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4113,10 +4104,10 @@
         <v>197</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4124,10 +4115,10 @@
         <v>198</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4135,10 +4126,10 @@
         <v>199</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4146,10 +4137,10 @@
         <v>200</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4157,16 +4148,16 @@
         <v>201</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4185,7 +4176,7 @@
       <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.18"/>
@@ -4193,24 +4184,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>9600</v>
@@ -4219,15 +4210,15 @@
         <v>13000</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2970</v>
@@ -4236,15 +4227,15 @@
         <v>11000</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">960/0.8</f>
@@ -4254,16 +4245,16 @@
         <v>8500</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4282,52 +4273,52 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="K1" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="L1" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>43</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>9450</v>
@@ -4336,30 +4327,30 @@
         <v>9355500</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>990</v>
       </c>
       <c r="H2" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="J2" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="K2" s="0" t="s">
         <v>84</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>44</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>2362.5</v>
@@ -4368,30 +4359,30 @@
         <v>6237000</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>2640</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>2362.5</v>
@@ -4400,30 +4391,30 @@
         <v>6237000</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>2640</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>44</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>787.4</v>
@@ -4432,30 +4423,30 @@
         <v>2078736</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>2640</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>787.4</v>
@@ -4464,30 +4455,30 @@
         <v>2078736</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>2640</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>45</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>284.990952380952</v>
@@ -4496,30 +4487,30 @@
         <v>3704882.38095238</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>13000</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I7" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="K7" s="0" t="s">
         <v>91</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="K7" s="0" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>839.973333333333</v>
@@ -4528,30 +4519,30 @@
         <v>11759626.6666667</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>14000</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>7874</v>
@@ -4560,30 +4551,30 @@
         <v>4724400</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>600</v>
       </c>
       <c r="H9" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="J9" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="I9" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>97</v>
-      </c>
       <c r="K9" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>7874</v>
@@ -4592,30 +4583,30 @@
         <v>4330700</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G10" s="0" t="n">
         <v>550</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I10" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="K10" s="0" t="s">
         <v>96</v>
-      </c>
-      <c r="J10" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="K10" s="0" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>50</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>51</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>2519.92</v>
@@ -4624,30 +4615,30 @@
         <v>21419320</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G11" s="0" t="n">
         <v>8500</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>53</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>28500</v>
@@ -4656,30 +4647,30 @@
         <v>8464500</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G12" s="0" t="n">
         <v>297</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J12" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="K12" s="0" t="s">
         <v>102</v>
-      </c>
-      <c r="K12" s="0" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>53</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>54</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>28500</v>
@@ -4688,30 +4679,30 @@
         <v>8778000</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G13" s="0" t="n">
         <v>308</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J13" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="K13" s="0" t="s">
         <v>103</v>
-      </c>
-      <c r="K13" s="0" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>55</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>5730.97826086957</v>
@@ -4720,30 +4711,30 @@
         <v>10716929.3478261</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G14" s="0" t="n">
         <v>1870</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>55</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>56</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>5730.97826086957</v>
@@ -4752,30 +4743,30 @@
         <v>13754347.826087</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G15" s="0" t="n">
         <v>2400</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>17800</v>
@@ -4784,30 +4775,30 @@
         <v>35244000</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G16" s="0" t="n">
         <v>1980</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J16" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="K16" s="0" t="s">
         <v>110</v>
-      </c>
-      <c r="K16" s="0" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>4628</v>
@@ -4816,30 +4807,30 @@
         <v>46280000</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G17" s="0" t="n">
         <v>10000</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>1725.23076923077</v>
@@ -4848,30 +4839,30 @@
         <v>18977538.4615385</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G18" s="0" t="n">
         <v>11000</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>511.379598662208</v>
@@ -4880,30 +4871,30 @@
         <v>5113795.98662208</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G19" s="0" t="n">
         <v>10000</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>1534.13879598662</v>
@@ -4912,28 +4903,28 @@
         <v>16875526.7558528</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G20" s="0" t="n">
         <v>11000</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4952,88 +4943,88 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.09"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>116</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5052,29 +5043,29 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>132</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5082,7 +5073,7 @@
         <v>186</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>34363.6356188246</v>
@@ -5105,7 +5096,7 @@
         <v>187</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>63</v>
@@ -5128,7 +5119,7 @@
         <v>188</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>2.99904761904762</v>
@@ -5151,7 +5142,7 @@
         <v>191</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>138.140350877193</v>
@@ -5174,7 +5165,7 @@
         <v>192</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>11579.4116429082</v>
@@ -5197,7 +5188,7 @@
         <v>193</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>29.9904761904762</v>
@@ -5220,7 +5211,7 @@
         <v>195</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>11728.3947395248</v>
@@ -5243,7 +5234,7 @@
         <v>196</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>66.9014084507042</v>
@@ -5266,7 +5257,7 @@
         <v>197</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>192.567567567568</v>
@@ -5289,7 +5280,7 @@
         <v>198</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>20.0384615384615</v>
@@ -5312,7 +5303,7 @@
         <v>199</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>3.17857142857143</v>
@@ -5332,8 +5323,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5352,105 +5343,105 @@
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>135</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>35244000</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>1746665.226</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B4" s="2" t="n">
         <f aca="false">555800.065+392749.215+110996.476</f>
         <v>1059545.756</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>678408.48</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>320398.308</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>1445.072</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>51393795.9866221</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
fix(employments): displaying employments details data only if provided
</commit_message>
<xml_diff>
--- a/data/xls/eco/VCA4D Coffee Ecuador Transfer.xlsx
+++ b/data/xls/eco/VCA4D Coffee Ecuador Transfer.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="171">
   <si>
     <t xml:space="preserve">Property</t>
   </si>
@@ -659,7 +659,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L2:L12 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -682,7 +682,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L2:L12 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -877,8 +877,8 @@
   </sheetPr>
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -927,7 +927,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>42</v>
       </c>
@@ -937,14 +937,26 @@
       <c r="C2" s="0" t="s">
         <v>158</v>
       </c>
+      <c r="D2" s="0" t="s">
+        <v>5</v>
+      </c>
       <c r="F2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>43</v>
       </c>
@@ -954,14 +966,26 @@
       <c r="C3" s="0" t="s">
         <v>158</v>
       </c>
+      <c r="D3" s="0" t="s">
+        <v>5</v>
+      </c>
       <c r="F3" s="2" t="n">
         <v>72.9696845159044</v>
       </c>
       <c r="G3" s="0" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>55</v>
       </c>
@@ -971,14 +995,26 @@
       <c r="C4" s="0" t="s">
         <v>158</v>
       </c>
+      <c r="D4" s="0" t="s">
+        <v>5</v>
+      </c>
       <c r="F4" s="2" t="n">
         <v>347.534453339202</v>
       </c>
       <c r="G4" s="0" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>49</v>
       </c>
@@ -988,14 +1024,26 @@
       <c r="C5" s="0" t="s">
         <v>158</v>
       </c>
+      <c r="D5" s="0" t="s">
+        <v>5</v>
+      </c>
       <c r="F5" s="2" t="n">
         <v>9.23970680434903</v>
       </c>
       <c r="G5" s="0" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>41</v>
       </c>
@@ -1005,14 +1053,26 @@
       <c r="C6" s="0" t="s">
         <v>158</v>
       </c>
+      <c r="D6" s="0" t="s">
+        <v>5</v>
+      </c>
       <c r="F6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G6" s="0" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>48</v>
       </c>
@@ -1022,14 +1082,26 @@
       <c r="C7" s="0" t="s">
         <v>158</v>
       </c>
+      <c r="D7" s="0" t="s">
+        <v>5</v>
+      </c>
       <c r="F7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G7" s="0" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>51</v>
       </c>
@@ -1039,14 +1111,26 @@
       <c r="C8" s="0" t="s">
         <v>158</v>
       </c>
+      <c r="D8" s="0" t="s">
+        <v>5</v>
+      </c>
       <c r="F8" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>47</v>
       </c>
@@ -1056,14 +1140,26 @@
       <c r="C9" s="0" t="s">
         <v>158</v>
       </c>
+      <c r="D9" s="0" t="s">
+        <v>5</v>
+      </c>
       <c r="F9" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H9" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>52</v>
       </c>
@@ -1073,14 +1169,26 @@
       <c r="C10" s="0" t="s">
         <v>158</v>
       </c>
+      <c r="D10" s="0" t="s">
+        <v>5</v>
+      </c>
       <c r="F10" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H10" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>53</v>
       </c>
@@ -1090,14 +1198,26 @@
       <c r="C11" s="0" t="s">
         <v>158</v>
       </c>
+      <c r="D11" s="0" t="s">
+        <v>5</v>
+      </c>
       <c r="F11" s="2" t="n">
         <v>14.2364470654456</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H11" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>54</v>
       </c>
@@ -1107,11 +1227,23 @@
       <c r="C12" s="0" t="s">
         <v>158</v>
       </c>
+      <c r="D12" s="0" t="s">
+        <v>5</v>
+      </c>
       <c r="F12" s="2" t="n">
         <v>49.8565051208285</v>
       </c>
       <c r="G12" s="0" t="s">
         <v>158</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1133,7 +1265,7 @@
   <dimension ref="A1:E145"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
+      <selection pane="topLeft" activeCell="A28" activeCellId="1" sqref="L2:L12 A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3622,7 +3754,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L2:L12 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3644,8 +3776,8 @@
   </sheetPr>
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="L2:L12 B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3893,7 +4025,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="L2:L12 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3957,12 +4089,13 @@
   </sheetPr>
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B20" activeCellId="1" sqref="L2:L12 B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32"/>
   </cols>
@@ -4173,7 +4306,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="1" sqref="L2:L12 E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4270,7 +4403,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L2:L12 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4940,7 +5073,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L2:L12 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5040,7 +5173,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L2:L12 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5340,7 +5473,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="1" sqref="L2:L12 C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
fix(data): coffee ecuador flows data
</commit_message>
<xml_diff>
--- a/data/xls/eco/VCA4D Coffee Ecuador Transfer.xlsx
+++ b/data/xls/eco/VCA4D Coffee Ecuador Transfer.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId2"/>
@@ -244,19 +244,19 @@
     <t xml:space="preserve">Buyer Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Volume</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exchang Value</t>
+    <t xml:space="preserve">Volume exchanged (kg Of product)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monetary value</t>
   </si>
   <si>
     <t xml:space="preserve">Relationship</t>
   </si>
   <si>
-    <t xml:space="preserve">Output</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price</t>
+    <t xml:space="preserve">Products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unitary price (local curency)</t>
   </si>
   <si>
     <t xml:space="preserve">Provider Function</t>
@@ -556,7 +556,7 @@
     <numFmt numFmtId="165" formatCode="#,##0"/>
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -578,6 +578,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -622,13 +628,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -659,7 +669,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L2:L12 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -682,7 +692,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L2:L12 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -877,8 +887,8 @@
   </sheetPr>
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2:L12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -931,7 +941,7 @@
       <c r="A2" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="3" t="n">
         <v>152.212275372031</v>
       </c>
       <c r="C2" s="0" t="s">
@@ -940,7 +950,7 @@
       <c r="D2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="3" t="n">
         <v>0</v>
       </c>
       <c r="G2" s="0" t="s">
@@ -960,7 +970,7 @@
       <c r="A3" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="3" t="n">
         <v>389.17165075149</v>
       </c>
       <c r="C3" s="0" t="s">
@@ -969,7 +979,7 @@
       <c r="D3" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="3" t="n">
         <v>72.9696845159044</v>
       </c>
       <c r="G3" s="0" t="s">
@@ -989,7 +999,7 @@
       <c r="A4" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="3" t="n">
         <v>1853.51708447574</v>
       </c>
       <c r="C4" s="0" t="s">
@@ -998,7 +1008,7 @@
       <c r="D4" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="3" t="n">
         <v>347.534453339202</v>
       </c>
       <c r="G4" s="0" t="s">
@@ -1018,7 +1028,7 @@
       <c r="A5" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="3" t="n">
         <v>49.2784362898615</v>
       </c>
       <c r="C5" s="0" t="s">
@@ -1027,7 +1037,7 @@
       <c r="D5" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="3" t="n">
         <v>9.23970680434903</v>
       </c>
       <c r="G5" s="0" t="s">
@@ -1047,7 +1057,7 @@
       <c r="A6" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="3" t="n">
         <v>0</v>
       </c>
       <c r="C6" s="0" t="s">
@@ -1056,7 +1066,7 @@
       <c r="D6" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="F6" s="3" t="n">
         <v>0</v>
       </c>
       <c r="G6" s="0" t="s">
@@ -1076,7 +1086,7 @@
       <c r="A7" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="3" t="n">
         <v>0</v>
       </c>
       <c r="C7" s="0" t="s">
@@ -1085,7 +1095,7 @@
       <c r="D7" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="3" t="n">
         <v>0</v>
       </c>
       <c r="G7" s="0" t="s">
@@ -1105,7 +1115,7 @@
       <c r="A8" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="3" t="n">
         <v>0</v>
       </c>
       <c r="C8" s="0" t="s">
@@ -1114,7 +1124,7 @@
       <c r="D8" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="3" t="n">
         <v>0</v>
       </c>
       <c r="G8" s="0" t="s">
@@ -1134,7 +1144,7 @@
       <c r="A9" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="3" t="n">
         <v>12.2791423001949</v>
       </c>
       <c r="C9" s="0" t="s">
@@ -1143,7 +1153,7 @@
       <c r="D9" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F9" s="3" t="n">
         <v>0</v>
       </c>
       <c r="G9" s="0" t="s">
@@ -1163,7 +1173,7 @@
       <c r="A10" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="3" t="n">
         <v>21.4084507042254</v>
       </c>
       <c r="C10" s="0" t="s">
@@ -1172,7 +1182,7 @@
       <c r="D10" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="2" t="n">
+      <c r="F10" s="3" t="n">
         <v>0</v>
       </c>
       <c r="G10" s="0" t="s">
@@ -1192,7 +1202,7 @@
       <c r="A11" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="3" t="n">
         <v>75.9277176823765</v>
       </c>
       <c r="C11" s="0" t="s">
@@ -1201,7 +1211,7 @@
       <c r="D11" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="2" t="n">
+      <c r="F11" s="3" t="n">
         <v>14.2364470654456</v>
       </c>
       <c r="G11" s="0" t="s">
@@ -1221,7 +1231,7 @@
       <c r="A12" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="3" t="n">
         <v>265.901360644419</v>
       </c>
       <c r="C12" s="0" t="s">
@@ -1230,7 +1240,7 @@
       <c r="D12" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="2" t="n">
+      <c r="F12" s="3" t="n">
         <v>49.8565051208285</v>
       </c>
       <c r="G12" s="0" t="s">
@@ -1265,7 +1275,7 @@
   <dimension ref="A1:E145"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A28" activeCellId="1" sqref="L2:L12 A28"/>
+      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3754,7 +3764,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L2:L12 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3777,7 +3787,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="L2:L12 B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4025,7 +4035,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="L2:L12 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4090,7 +4100,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="1" sqref="L2:L12 B20"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4306,7 +4316,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="1" sqref="L2:L12 E5"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4402,13 +4412,26 @@
   </sheetPr>
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L2:L12 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="6.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="7.64"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>68</v>
       </c>
@@ -4418,7 +4441,7 @@
       <c r="C1" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E1" s="0" t="s">
@@ -4427,7 +4450,7 @@
       <c r="F1" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="2" t="s">
         <v>74</v>
       </c>
       <c r="H1" s="0" t="s">
@@ -5073,7 +5096,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L2:L12 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5173,7 +5196,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L2:L12 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5473,7 +5496,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="1" sqref="L2:L12 C9"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5497,10 +5520,10 @@
       <c r="A2" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="3" t="n">
         <v>35244000</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>136</v>
       </c>
     </row>
@@ -5508,10 +5531,10 @@
       <c r="A3" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="3" t="n">
         <v>1746665.226</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>136</v>
       </c>
     </row>
@@ -5519,11 +5542,11 @@
       <c r="A4" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="3" t="n">
         <f aca="false">555800.065+392749.215+110996.476</f>
         <v>1059545.756</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>136</v>
       </c>
     </row>
@@ -5531,10 +5554,10 @@
       <c r="A5" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="3" t="n">
         <v>678408.48</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>136</v>
       </c>
     </row>
@@ -5542,10 +5565,10 @@
       <c r="A6" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="3" t="n">
         <v>320398.308</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>136</v>
       </c>
     </row>
@@ -5553,10 +5576,10 @@
       <c r="A7" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="3" t="n">
         <v>1445.072</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>136</v>
       </c>
     </row>
@@ -5564,10 +5587,10 @@
       <c r="A8" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="3" t="n">
         <v>51393795.9866221</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>143</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed excel ecuador coffee eco
</commit_message>
<xml_diff>
--- a/data/xls/eco/VCA4D Coffee Ecuador Transfer.xlsx
+++ b/data/xls/eco/VCA4D Coffee Ecuador Transfer.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="170">
   <si>
     <t xml:space="preserve">Property</t>
   </si>
@@ -472,9 +472,6 @@
     <t xml:space="preserve">Receiver Name</t>
   </si>
   <si>
-    <t xml:space="preserve">value (local currency)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Land owners (land fees)</t>
   </si>
   <si>
@@ -484,7 +481,7 @@
     <t xml:space="preserve">Employees (wages)</t>
   </si>
   <si>
-    <t xml:space="preserve">Financial institutions (interests On loans)</t>
+    <t xml:space="preserve">Financial institutions (interests on loans)</t>
   </si>
   <si>
     <t xml:space="preserve">Government (taxes - subsidies)</t>
@@ -556,7 +553,7 @@
     <numFmt numFmtId="165" formatCode="#,##0"/>
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -578,12 +575,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -637,7 +628,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -691,11 +682,15 @@
   </sheetPr>
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.14"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -705,7 +700,7 @@
         <v>145</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -831,7 +826,7 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>0</v>
@@ -839,7 +834,7 @@
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>11979570.8198526</v>
@@ -847,7 +842,7 @@
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>15651653.0923037</v>
@@ -855,7 +850,7 @@
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>0</v>
@@ -863,7 +858,7 @@
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>174805.067685938</v>
@@ -888,7 +883,7 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -901,37 +896,37 @@
         <v>127</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>2</v>
@@ -945,25 +940,13 @@
         <v>152.212275372031</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>5</v>
+        <v>157</v>
       </c>
       <c r="F2" s="3" t="n">
         <v>0</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>5</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -974,25 +957,13 @@
         <v>389.17165075149</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>5</v>
+        <v>157</v>
       </c>
       <c r="F3" s="3" t="n">
         <v>72.9696845159044</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>5</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1003,25 +974,13 @@
         <v>1853.51708447574</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>5</v>
+        <v>157</v>
       </c>
       <c r="F4" s="3" t="n">
         <v>347.534453339202</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>5</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1032,25 +991,13 @@
         <v>49.2784362898615</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>5</v>
+        <v>157</v>
       </c>
       <c r="F5" s="3" t="n">
         <v>9.23970680434903</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="L5" s="0" t="s">
-        <v>5</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1061,25 +1008,13 @@
         <v>0</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>5</v>
+        <v>157</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>0</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="L6" s="0" t="s">
-        <v>5</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1090,25 +1025,13 @@
         <v>0</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>5</v>
+        <v>157</v>
       </c>
       <c r="F7" s="3" t="n">
         <v>0</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="L7" s="0" t="s">
-        <v>5</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1119,25 +1042,13 @@
         <v>0</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>5</v>
+        <v>157</v>
       </c>
       <c r="F8" s="3" t="n">
         <v>0</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="J8" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="L8" s="0" t="s">
-        <v>5</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1148,25 +1059,13 @@
         <v>12.2791423001949</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>5</v>
+        <v>157</v>
       </c>
       <c r="F9" s="3" t="n">
         <v>0</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="L9" s="0" t="s">
-        <v>5</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1177,25 +1076,13 @@
         <v>21.4084507042254</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>5</v>
+        <v>157</v>
       </c>
       <c r="F10" s="3" t="n">
         <v>0</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="J10" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="L10" s="0" t="s">
-        <v>5</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1206,25 +1093,13 @@
         <v>75.9277176823765</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>5</v>
+        <v>157</v>
       </c>
       <c r="F11" s="3" t="n">
         <v>14.2364470654456</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="L11" s="0" t="s">
-        <v>5</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1235,25 +1110,13 @@
         <v>265.901360644419</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>5</v>
+        <v>157</v>
       </c>
       <c r="F12" s="3" t="n">
         <v>49.8565051208285</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="J12" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="L12" s="0" t="s">
-        <v>5</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1288,10 +1151,10 @@
         <v>40</v>
       </c>
       <c r="C1" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" s="0" t="s">
         <v>159</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>160</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>1</v>
@@ -1305,10 +1168,10 @@
         <v>41</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>2654590.92547677</v>
@@ -1322,10 +1185,10 @@
         <v>42</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>74503.0838454333</v>
@@ -1339,10 +1202,10 @@
         <v>43</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>4199866.66666666</v>
@@ -1356,10 +1219,10 @@
         <v>44</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>0</v>
@@ -1373,10 +1236,10 @@
         <v>46</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>0</v>
@@ -1390,10 +1253,10 @@
         <v>47</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>44941.6607747998</v>
@@ -1407,10 +1270,10 @@
         <v>48</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>1367335.54657768</v>
@@ -1424,10 +1287,10 @@
         <v>49</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>277491.19047619</v>
@@ -1441,10 +1304,10 @@
         <v>50</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>0</v>
@@ -1458,10 +1321,10 @@
         <v>51</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>2125537.02607567</v>
@@ -1475,10 +1338,10 @@
         <v>52</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>16932.4121811021</v>
@@ -1492,10 +1355,10 @@
         <v>53</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>83414.77565273</v>
@@ -1509,10 +1372,10 @@
         <v>54</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>121315.391657326</v>
@@ -1526,10 +1389,10 @@
         <v>55</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>1013642.14046823</v>
@@ -1543,10 +1406,10 @@
         <v>57</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>0</v>
@@ -1560,10 +1423,10 @@
         <v>58</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>0</v>
@@ -1577,10 +1440,10 @@
         <v>41</v>
       </c>
       <c r="C18" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="D18" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>162</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>721636.363636364</v>
@@ -1594,10 +1457,10 @@
         <v>42</v>
       </c>
       <c r="C19" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="D19" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>162</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>14908632.0347334</v>
@@ -1611,10 +1474,10 @@
         <v>43</v>
       </c>
       <c r="C20" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="D20" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>162</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>8409723.01619047</v>
@@ -1628,10 +1491,10 @@
         <v>44</v>
       </c>
       <c r="C21" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="D21" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>162</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>0</v>
@@ -1645,10 +1508,10 @@
         <v>46</v>
       </c>
       <c r="C22" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="D22" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>162</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>0</v>
@@ -1662,10 +1525,10 @@
         <v>47</v>
       </c>
       <c r="C23" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="D23" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>162</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>4330700</v>
@@ -1679,10 +1542,10 @@
         <v>48</v>
       </c>
       <c r="C24" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="D24" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>162</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>65134.1911764706</v>
@@ -1696,10 +1559,10 @@
         <v>49</v>
       </c>
       <c r="C25" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="D25" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>162</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>8315736</v>
@@ -1713,10 +1576,10 @@
         <v>50</v>
       </c>
       <c r="C26" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="D26" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>162</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>0</v>
@@ -1730,10 +1593,10 @@
         <v>51</v>
       </c>
       <c r="C27" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="D27" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>162</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>237500</v>
@@ -1747,10 +1610,10 @@
         <v>52</v>
       </c>
       <c r="C28" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="D28" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>162</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>8466667.60548068</v>
@@ -1764,10 +1627,10 @@
         <v>53</v>
       </c>
       <c r="C29" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="D29" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>162</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>9241024.29796303</v>
@@ -1781,10 +1644,10 @@
         <v>54</v>
       </c>
       <c r="C30" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="D30" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>162</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>11431890.9006974</v>
@@ -1798,10 +1661,10 @@
         <v>55</v>
       </c>
       <c r="C31" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="D31" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>162</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>84951227.5965719</v>
@@ -1815,10 +1678,10 @@
         <v>57</v>
       </c>
       <c r="C32" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="D32" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>162</v>
       </c>
       <c r="E32" s="0" t="n">
         <v>0</v>
@@ -1832,10 +1695,10 @@
         <v>58</v>
       </c>
       <c r="C33" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="D33" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>162</v>
       </c>
       <c r="E33" s="0" t="n">
         <v>0</v>
@@ -1849,10 +1712,10 @@
         <v>41</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E34" s="0" t="n">
         <v>0</v>
@@ -1866,10 +1729,10 @@
         <v>42</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>0</v>
@@ -1883,10 +1746,10 @@
         <v>43</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E36" s="0" t="n">
         <v>0</v>
@@ -1900,10 +1763,10 @@
         <v>44</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E37" s="0" t="n">
         <v>0</v>
@@ -1917,10 +1780,10 @@
         <v>46</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E38" s="0" t="n">
         <v>0</v>
@@ -1934,10 +1797,10 @@
         <v>47</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E39" s="0" t="n">
         <v>0</v>
@@ -1951,10 +1814,10 @@
         <v>48</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E40" s="0" t="n">
         <v>0</v>
@@ -1968,10 +1831,10 @@
         <v>49</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E41" s="0" t="n">
         <v>0</v>
@@ -1985,10 +1848,10 @@
         <v>50</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E42" s="0" t="n">
         <v>0</v>
@@ -2002,10 +1865,10 @@
         <v>51</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E43" s="0" t="n">
         <v>0</v>
@@ -2019,10 +1882,10 @@
         <v>52</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E44" s="0" t="n">
         <v>0</v>
@@ -2036,10 +1899,10 @@
         <v>53</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E45" s="0" t="n">
         <v>0</v>
@@ -2053,10 +1916,10 @@
         <v>54</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E46" s="0" t="n">
         <v>0</v>
@@ -2070,10 +1933,10 @@
         <v>55</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E47" s="0" t="n">
         <v>0</v>
@@ -2087,10 +1950,10 @@
         <v>57</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E48" s="0" t="n">
         <v>0</v>
@@ -2104,10 +1967,10 @@
         <v>58</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E49" s="0" t="n">
         <v>0</v>
@@ -2121,10 +1984,10 @@
         <v>41</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E50" s="0" t="n">
         <v>0</v>
@@ -2138,10 +2001,10 @@
         <v>42</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E51" s="0" t="n">
         <v>0</v>
@@ -2155,10 +2018,10 @@
         <v>43</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E52" s="0" t="n">
         <v>0</v>
@@ -2172,10 +2035,10 @@
         <v>44</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E53" s="0" t="n">
         <v>0</v>
@@ -2189,10 +2052,10 @@
         <v>46</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E54" s="0" t="n">
         <v>0</v>
@@ -2206,10 +2069,10 @@
         <v>47</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E55" s="0" t="n">
         <v>0</v>
@@ -2223,10 +2086,10 @@
         <v>48</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E56" s="0" t="n">
         <v>0</v>
@@ -2240,10 +2103,10 @@
         <v>49</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E57" s="0" t="n">
         <v>0</v>
@@ -2257,10 +2120,10 @@
         <v>50</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E58" s="0" t="n">
         <v>0</v>
@@ -2274,10 +2137,10 @@
         <v>51</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E59" s="0" t="n">
         <v>0</v>
@@ -2291,10 +2154,10 @@
         <v>52</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E60" s="0" t="n">
         <v>0</v>
@@ -2308,10 +2171,10 @@
         <v>53</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E61" s="0" t="n">
         <v>0</v>
@@ -2325,10 +2188,10 @@
         <v>54</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E62" s="0" t="n">
         <v>0</v>
@@ -2342,10 +2205,10 @@
         <v>55</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E63" s="0" t="n">
         <v>0</v>
@@ -2359,10 +2222,10 @@
         <v>57</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E64" s="0" t="n">
         <v>0</v>
@@ -2376,10 +2239,10 @@
         <v>58</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E65" s="0" t="n">
         <v>0</v>
@@ -2393,10 +2256,10 @@
         <v>41</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E66" s="0" t="n">
         <v>5841818.16543232</v>
@@ -2410,10 +2273,10 @@
         <v>42</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E67" s="0" t="n">
         <v>729927.234903794</v>
@@ -2427,10 +2290,10 @@
         <v>43</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E68" s="0" t="n">
         <v>621430.271428574</v>
@@ -2444,10 +2307,10 @@
         <v>44</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E69" s="0" t="n">
         <v>0</v>
@@ -2461,10 +2324,10 @@
         <v>46</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E70" s="0" t="n">
         <v>0</v>
@@ -2478,10 +2341,10 @@
         <v>47</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E71" s="0" t="n">
         <v>293502.198874323</v>
@@ -2495,10 +2358,10 @@
         <v>48</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E72" s="0" t="n">
         <v>2724539.08577526</v>
@@ -2512,10 +2375,10 @@
         <v>49</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E73" s="0" t="n">
         <v>12271410.4190476</v>
@@ -2529,10 +2392,10 @@
         <v>50</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E74" s="0" t="n">
         <v>0</v>
@@ -2546,10 +2409,10 @@
         <v>51</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E75" s="0" t="n">
         <v>6101463.23162832</v>
@@ -2563,10 +2426,10 @@
         <v>52</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E76" s="0" t="n">
         <v>136646.465550007</v>
@@ -2580,10 +2443,10 @@
         <v>53</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E77" s="0" t="n">
         <v>830641.433828549</v>
@@ -2597,10 +2460,10 @@
         <v>54</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E78" s="0" t="n">
         <v>679657.000221048</v>
@@ -2614,10 +2477,10 @@
         <v>55</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E79" s="0" t="n">
         <v>25846547.4870402</v>
@@ -2631,10 +2494,10 @@
         <v>57</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E80" s="0" t="n">
         <v>0</v>
@@ -2648,10 +2511,10 @@
         <v>58</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E81" s="0" t="n">
         <v>0</v>
@@ -2665,10 +2528,10 @@
         <v>41</v>
       </c>
       <c r="C82" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="D82" s="0" t="s">
         <v>166</v>
-      </c>
-      <c r="D82" s="0" t="s">
-        <v>167</v>
       </c>
       <c r="E82" s="0" t="n">
         <v>9355500</v>
@@ -2682,10 +2545,10 @@
         <v>42</v>
       </c>
       <c r="C83" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="D83" s="0" t="s">
         <v>166</v>
-      </c>
-      <c r="D83" s="0" t="s">
-        <v>167</v>
       </c>
       <c r="E83" s="0" t="n">
         <v>16631472</v>
@@ -2699,10 +2562,10 @@
         <v>43</v>
       </c>
       <c r="C84" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="D84" s="0" t="s">
         <v>166</v>
-      </c>
-      <c r="D84" s="0" t="s">
-        <v>167</v>
       </c>
       <c r="E84" s="0" t="n">
         <v>15464509.047619</v>
@@ -2716,10 +2579,10 @@
         <v>44</v>
       </c>
       <c r="C85" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="D85" s="0" t="s">
         <v>166</v>
-      </c>
-      <c r="D85" s="0" t="s">
-        <v>167</v>
       </c>
       <c r="E85" s="0" t="n">
         <v>0</v>
@@ -2733,10 +2596,10 @@
         <v>46</v>
       </c>
       <c r="C86" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="D86" s="0" t="s">
         <v>166</v>
-      </c>
-      <c r="D86" s="0" t="s">
-        <v>167</v>
       </c>
       <c r="E86" s="0" t="n">
         <v>0</v>
@@ -2750,10 +2613,10 @@
         <v>47</v>
       </c>
       <c r="C87" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="D87" s="0" t="s">
         <v>166</v>
-      </c>
-      <c r="D87" s="0" t="s">
-        <v>167</v>
       </c>
       <c r="E87" s="0" t="n">
         <v>4724400</v>
@@ -2767,10 +2630,10 @@
         <v>48</v>
       </c>
       <c r="C88" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="D88" s="0" t="s">
         <v>166</v>
-      </c>
-      <c r="D88" s="0" t="s">
-        <v>167</v>
       </c>
       <c r="E88" s="0" t="n">
         <v>4330700</v>
@@ -2784,10 +2647,10 @@
         <v>49</v>
       </c>
       <c r="C89" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="D89" s="0" t="s">
         <v>166</v>
-      </c>
-      <c r="D89" s="0" t="s">
-        <v>167</v>
       </c>
       <c r="E89" s="0" t="n">
         <v>21419320</v>
@@ -2801,10 +2664,10 @@
         <v>50</v>
       </c>
       <c r="C90" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="D90" s="0" t="s">
         <v>166</v>
-      </c>
-      <c r="D90" s="0" t="s">
-        <v>167</v>
       </c>
       <c r="E90" s="0" t="n">
         <v>0</v>
@@ -2818,10 +2681,10 @@
         <v>51</v>
       </c>
       <c r="C91" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="D91" s="0" t="s">
         <v>166</v>
-      </c>
-      <c r="D91" s="0" t="s">
-        <v>167</v>
       </c>
       <c r="E91" s="0" t="n">
         <v>8464500.25770399</v>
@@ -2835,10 +2698,10 @@
         <v>52</v>
       </c>
       <c r="C92" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="D92" s="0" t="s">
         <v>166</v>
-      </c>
-      <c r="D92" s="0" t="s">
-        <v>167</v>
       </c>
       <c r="E92" s="0" t="n">
         <v>8778000</v>
@@ -2852,10 +2715,10 @@
         <v>53</v>
       </c>
       <c r="C93" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="D93" s="0" t="s">
         <v>166</v>
-      </c>
-      <c r="D93" s="0" t="s">
-        <v>167</v>
       </c>
       <c r="E93" s="0" t="n">
         <v>11000380.4347826</v>
@@ -2869,10 +2732,10 @@
         <v>54</v>
       </c>
       <c r="C94" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="D94" s="0" t="s">
         <v>166</v>
-      </c>
-      <c r="D94" s="0" t="s">
-        <v>167</v>
       </c>
       <c r="E94" s="0" t="n">
         <v>13754347.826087</v>
@@ -2886,10 +2749,10 @@
         <v>55</v>
       </c>
       <c r="C95" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="D95" s="0" t="s">
         <v>166</v>
-      </c>
-      <c r="D95" s="0" t="s">
-        <v>167</v>
       </c>
       <c r="E95" s="0" t="n">
         <v>122490861.204013</v>
@@ -2903,10 +2766,10 @@
         <v>57</v>
       </c>
       <c r="C96" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="D96" s="0" t="s">
         <v>166</v>
-      </c>
-      <c r="D96" s="0" t="s">
-        <v>167</v>
       </c>
       <c r="E96" s="0" t="n">
         <v>0</v>
@@ -2920,10 +2783,10 @@
         <v>58</v>
       </c>
       <c r="C97" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="D97" s="0" t="s">
         <v>166</v>
-      </c>
-      <c r="D97" s="0" t="s">
-        <v>167</v>
       </c>
       <c r="E97" s="0" t="n">
         <v>0</v>
@@ -2937,10 +2800,10 @@
         <v>41</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E98" s="0" t="n">
         <v>0</v>
@@ -2954,10 +2817,10 @@
         <v>42</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E99" s="0" t="n">
         <v>0</v>
@@ -2971,10 +2834,10 @@
         <v>43</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E100" s="0" t="n">
         <v>0</v>
@@ -2988,10 +2851,10 @@
         <v>44</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E101" s="0" t="n">
         <v>0</v>
@@ -3005,10 +2868,10 @@
         <v>46</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E102" s="0" t="n">
         <v>0</v>
@@ -3022,10 +2885,10 @@
         <v>47</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E103" s="0" t="n">
         <v>0</v>
@@ -3039,10 +2902,10 @@
         <v>48</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E104" s="0" t="n">
         <v>0</v>
@@ -3056,10 +2919,10 @@
         <v>49</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D105" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E105" s="0" t="n">
         <v>0</v>
@@ -3073,10 +2936,10 @@
         <v>50</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D106" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E106" s="0" t="n">
         <v>0</v>
@@ -3090,10 +2953,10 @@
         <v>51</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D107" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E107" s="0" t="n">
         <v>0</v>
@@ -3107,10 +2970,10 @@
         <v>52</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D108" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E108" s="0" t="n">
         <v>0</v>
@@ -3124,10 +2987,10 @@
         <v>53</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E109" s="0" t="n">
         <v>0</v>
@@ -3141,10 +3004,10 @@
         <v>54</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E110" s="0" t="n">
         <v>0</v>
@@ -3158,10 +3021,10 @@
         <v>55</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E111" s="0" t="n">
         <v>0</v>
@@ -3175,10 +3038,10 @@
         <v>57</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E112" s="0" t="n">
         <v>0</v>
@@ -3192,10 +3055,10 @@
         <v>58</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E113" s="0" t="n">
         <v>0</v>
@@ -3209,10 +3072,10 @@
         <v>41</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E114" s="0" t="n">
         <v>0</v>
@@ -3226,10 +3089,10 @@
         <v>42</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E115" s="0" t="n">
         <v>0</v>
@@ -3243,10 +3106,10 @@
         <v>43</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E116" s="0" t="n">
         <v>29999.0476190476</v>
@@ -3260,10 +3123,10 @@
         <v>44</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E117" s="0" t="n">
         <v>0</v>
@@ -3277,10 +3140,10 @@
         <v>46</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D118" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E118" s="0" t="n">
         <v>0</v>
@@ -3294,10 +3157,10 @@
         <v>47</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E119" s="0" t="n">
         <v>0</v>
@@ -3311,10 +3174,10 @@
         <v>48</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D120" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E120" s="0" t="n">
         <v>0</v>
@@ -3328,10 +3191,10 @@
         <v>49</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D121" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E121" s="0" t="n">
         <v>0</v>
@@ -3345,10 +3208,10 @@
         <v>50</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D122" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E122" s="0" t="n">
         <v>0</v>
@@ -3362,10 +3225,10 @@
         <v>51</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D123" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E123" s="0" t="n">
         <v>0</v>
@@ -3379,10 +3242,10 @@
         <v>52</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D124" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E124" s="0" t="n">
         <v>0</v>
@@ -3396,10 +3259,10 @@
         <v>53</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D125" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E125" s="0" t="n">
         <v>0</v>
@@ -3413,10 +3276,10 @@
         <v>54</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D126" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E126" s="0" t="n">
         <v>0</v>
@@ -3430,10 +3293,10 @@
         <v>55</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D127" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E127" s="0" t="n">
         <v>144806.02006689</v>
@@ -3447,10 +3310,10 @@
         <v>57</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D128" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E128" s="0" t="n">
         <v>0</v>
@@ -3464,10 +3327,10 @@
         <v>58</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D129" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E129" s="0" t="n">
         <v>0</v>
@@ -3481,10 +3344,10 @@
         <v>41</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D130" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E130" s="0" t="n">
         <v>0</v>
@@ -3498,10 +3361,10 @@
         <v>42</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D131" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E131" s="0" t="n">
         <v>684955.239174139</v>
@@ -3515,10 +3378,10 @@
         <v>43</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D132" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E132" s="0" t="n">
         <v>2189090.50285714</v>
@@ -3532,10 +3395,10 @@
         <v>44</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D133" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E133" s="0" t="n">
         <v>0</v>
@@ -3549,10 +3412,10 @@
         <v>46</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D134" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E134" s="0" t="n">
         <v>0</v>
@@ -3566,10 +3429,10 @@
         <v>47</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D135" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E135" s="0" t="n">
         <v>55256.1403508772</v>
@@ -3583,10 +3446,10 @@
         <v>48</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D136" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E136" s="0" t="n">
         <v>0</v>
@@ -3600,10 +3463,10 @@
         <v>49</v>
       </c>
       <c r="C137" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D137" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E137" s="0" t="n">
         <v>277191.2</v>
@@ -3617,10 +3480,10 @@
         <v>50</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D138" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E138" s="0" t="n">
         <v>0</v>
@@ -3634,10 +3497,10 @@
         <v>51</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D139" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E139" s="0" t="n">
         <v>0</v>
@@ -3651,10 +3514,10 @@
         <v>52</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D140" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E140" s="0" t="n">
         <v>96338.0281690141</v>
@@ -3668,10 +3531,10 @@
         <v>53</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D141" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E141" s="0" t="n">
         <v>427093.40559918</v>
@@ -3685,10 +3548,10 @@
         <v>54</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D142" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E142" s="0" t="n">
         <v>1495695.13133726</v>
@@ -3702,10 +3565,10 @@
         <v>55</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D143" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E143" s="0" t="n">
         <v>10426033.4448161</v>
@@ -3719,10 +3582,10 @@
         <v>57</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D144" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E144" s="0" t="n">
         <v>0</v>
@@ -3736,10 +3599,10 @@
         <v>58</v>
       </c>
       <c r="C145" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D145" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E145" s="0" t="n">
         <v>0</v>
@@ -3787,7 +3650,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4412,16 +4275,17 @@
   </sheetPr>
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="18.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.23"/>

</xml_diff>